<commit_message>
Biryani From Garuranga P updates by comparing with everest masala
</commit_message>
<xml_diff>
--- a/rice/Biryani from Gauranga Prabhu.xlsx
+++ b/rice/Biryani from Gauranga Prabhu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TranscendCard/sourcetree/nandini_recipies/rice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B66A96-6A8E-3B49-BFE9-FB230AA1217A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E7ADFC-3013-3C41-9F26-EA28B7C24EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{134C7825-DF8B-42D3-A51C-71C91B0E6488}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{134C7825-DF8B-42D3-A51C-71C91B0E6488}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Item name</t>
   </si>
@@ -134,9 +134,6 @@
     <t>kashmiri chilli powder</t>
   </si>
   <si>
-    <t>Biryani Masala</t>
-  </si>
-  <si>
     <t>Haldi</t>
   </si>
   <si>
@@ -147,6 +144,18 @@
   </si>
   <si>
     <t>Recipe seems to be wrong</t>
+  </si>
+  <si>
+    <t>Rice in grams</t>
+  </si>
+  <si>
+    <t>grams</t>
+  </si>
+  <si>
+    <t>Everest Biryani Masala</t>
+  </si>
+  <si>
+    <t>Bhajan se bhojan</t>
   </si>
 </sst>
 </file>
@@ -215,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +262,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,8 +287,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D76ED776-8104-432C-B917-1D930E70AF60}" name="Table1" displayName="Table1" ref="A1:F27" totalsRowShown="0">
-  <autoFilter ref="A1:F27" xr:uid="{12D95053-9C3E-4819-B2F6-1CB5C1FDDA15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D76ED776-8104-432C-B917-1D930E70AF60}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0">
+  <autoFilter ref="A1:F28" xr:uid="{12D95053-9C3E-4819-B2F6-1CB5C1FDDA15}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BD6E7EDD-66B1-4838-AD7A-A2AA04EF5520}" name="Item name"/>
     <tableColumn id="2" xr3:uid="{80E22383-2B6C-411A-A07C-2DA040A14090}" name="Daily recipe" dataDxfId="0">
@@ -588,25 +600,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E1998A-25FC-42BE-BFFC-DAF05717235E}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,13 +645,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -651,411 +665,454 @@
         <v>14</v>
       </c>
       <c r="B3" s="14">
-        <f t="shared" ref="B3:B21" si="0">(E3/F3)*D3</f>
-        <v>0.93100000000000005</v>
+        <f t="shared" ref="B3:B22" si="0">(E3/F3)*D3</f>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <v>1.33</v>
       </c>
       <c r="F3" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="15">
+        <f>(E4/F4)*D4</f>
+        <v>225.56390977443607</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>300</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5">
-        <f t="shared" si="0"/>
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="B5" s="5">
+        <f t="shared" si="0"/>
+        <v>3.007518796992481</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
         <v>4</v>
       </c>
-      <c r="F4" s="1">
-        <v>5</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="F5" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="11">
-        <f t="shared" si="0"/>
-        <v>2.9750000000000001</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="B6" s="11">
+        <f t="shared" si="0"/>
+        <v>3.1954887218045109</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
         <v>4.25</v>
       </c>
-      <c r="F5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5">
-        <f t="shared" si="0"/>
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.75</v>
-      </c>
       <c r="F6" s="1">
-        <v>5</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>9</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5">
         <f t="shared" si="0"/>
-        <v>0.52500000000000002</v>
+        <v>0.56390977443609025</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>0.75</v>
       </c>
       <c r="F7" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.56390977443609025</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>5</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="B10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="F10" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.56390977443609025</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.33</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="14">
-        <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.93100000000000005</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="14">
+        <f t="shared" si="0"/>
+        <v>0.37593984962406013</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>1.33</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" si="0"/>
-        <v>0.23100000000000001</v>
+        <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>0.33</v>
+        <v>1.33</v>
       </c>
       <c r="F14" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
+        <v>0.24812030075187969</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="F15" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5037593984962405</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5">
-        <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="14">
+        <f t="shared" si="0"/>
+        <v>0.37593984962406013</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
         <v>0.5</v>
       </c>
-      <c r="F16" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="F17" s="1">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="5">
-        <f t="shared" si="0"/>
-        <v>0.17500000000000002</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="F17" s="1">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="B18" s="5">
         <f t="shared" si="0"/>
-        <v>2.1</v>
+        <v>0.37593984962406013</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F18" s="1">
-        <v>5</v>
+        <v>1.33</v>
+      </c>
+      <c r="G18">
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5">
-        <f t="shared" si="0"/>
-        <v>0.46200000000000002</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="14">
+        <f t="shared" si="0"/>
+        <v>1.5037593984962405</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>0.66</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1">
-        <v>5</v>
+        <v>1.33</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
+        <v>0.49624060150375937</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D20" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>0.5</v>
+        <v>0.66</v>
       </c>
       <c r="F20" s="1">
-        <v>5</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
+        <v>0.37593984962406013</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F21" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>